<commit_message>
Chegando na primeira versão
</commit_message>
<xml_diff>
--- a/Python_ENEL_Anexo_C_Base_16092022.xlsx
+++ b/Python_ENEL_Anexo_C_Base_16092022.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24729"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25601"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\DOWNLOADS\DEV SINERGIA\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PC 24\DEV SINERGIA\SIN.ENEL V1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2428E21A-2C37-4C60-BD32-944369DB968D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1266FDAA-ABA7-4B02-A577-19F67B66D138}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20640" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="8520" yWindow="1815" windowWidth="28800" windowHeight="11310" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Plan1" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="94">
   <si>
     <t>Código da UC: NOVA</t>
   </si>
@@ -189,9 +189,6 @@
     <t>Cidade: $CidadeEnel</t>
   </si>
   <si>
-    <t>Nº:  $NumeroEnel</t>
-  </si>
-  <si>
     <t>CEP: $CepEnel</t>
   </si>
   <si>
@@ -204,12 +201,6 @@
     <t>CNPJ/CPF: $CNPJ</t>
   </si>
   <si>
-    <t xml:space="preserve">Localização em coordenadas ( Latitude , Longitude) : </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> $CoordenadasGD</t>
-  </si>
-  <si>
     <t>outro: $PotenciaTransformador</t>
   </si>
   <si>
@@ -270,15 +261,6 @@
     <t>bifásica     |  |</t>
   </si>
   <si>
-    <t>Nome/Procurador Legal:  $Solicitante</t>
-  </si>
-  <si>
-    <t>Telefone: $TelefoneSolicitante</t>
-  </si>
-  <si>
-    <t>E-mail: $EmailSolicitante</t>
-  </si>
-  <si>
     <t xml:space="preserve">ART do Responsável Técnico pelo projeto elétrico e instalação do sistema de minigeração                                   </t>
   </si>
   <si>
@@ -313,6 +295,21 @@
   </si>
   <si>
     <t>Potência instalada de geração (kW): $QuantidadeKwp</t>
+  </si>
+  <si>
+    <t>Nome/Procurador Legal:  $RepresentanteLegalUm</t>
+  </si>
+  <si>
+    <t>Telefone: $TelefoneCelularRepresentanteLegalUm</t>
+  </si>
+  <si>
+    <t>E-mail: $EmailRepresentanteLegalUm</t>
+  </si>
+  <si>
+    <t>Nº:  $NrEnel</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Localização em coordenadas ( Latitude , Longitude) :  $CoordenadasGD </t>
   </si>
 </sst>
 </file>
@@ -922,8 +919,8 @@
   </sheetPr>
   <dimension ref="A1:L54"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="F23" sqref="F23"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="I11" sqref="I11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" zeroHeight="1" x14ac:dyDescent="0.25"/>
@@ -931,7 +928,8 @@
     <col min="1" max="3" width="9.140625" style="1" customWidth="1"/>
     <col min="4" max="4" width="12.42578125" style="1" customWidth="1"/>
     <col min="5" max="5" width="10.85546875" style="1" customWidth="1"/>
-    <col min="6" max="12" width="9.140625" style="1" customWidth="1"/>
+    <col min="6" max="6" width="7.140625" style="1" customWidth="1"/>
+    <col min="7" max="12" width="9.140625" style="1" customWidth="1"/>
     <col min="13" max="16384" width="9.140625" style="1" hidden="1"/>
   </cols>
   <sheetData>
@@ -969,12 +967,12 @@
       </c>
       <c r="C5" s="3"/>
       <c r="D5" s="4" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="E5" s="3"/>
       <c r="F5" s="3"/>
       <c r="G5" s="1" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="H5" s="4"/>
       <c r="J5" s="9" t="s">
@@ -1007,11 +1005,11 @@
       <c r="E7" s="3"/>
       <c r="F7" s="3"/>
       <c r="G7" s="3" t="s">
-        <v>53</v>
+        <v>92</v>
       </c>
       <c r="H7" s="3"/>
       <c r="I7" s="3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="J7" s="3"/>
       <c r="K7" s="5"/>
@@ -1034,7 +1032,7 @@
     </row>
     <row r="9" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B9" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C9" s="7"/>
       <c r="D9" s="3"/>
@@ -1048,7 +1046,7 @@
     </row>
     <row r="10" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B10" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C10" s="3"/>
       <c r="D10" s="3"/>
@@ -1064,7 +1062,7 @@
     </row>
     <row r="11" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B11" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C11" s="3"/>
       <c r="D11" s="3"/>
@@ -1092,15 +1090,13 @@
     </row>
     <row r="13" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B13" s="6" t="s">
-        <v>58</v>
+        <v>93</v>
       </c>
       <c r="C13" s="3"/>
       <c r="D13" s="3"/>
       <c r="E13" s="3"/>
       <c r="F13" s="3"/>
-      <c r="G13" s="3" t="s">
-        <v>59</v>
-      </c>
+      <c r="G13" s="3"/>
       <c r="H13" s="3"/>
       <c r="I13" s="3"/>
       <c r="J13" s="3"/>
@@ -1108,7 +1104,7 @@
     </row>
     <row r="14" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B14" s="2" t="s">
-        <v>93</v>
+        <v>87</v>
       </c>
       <c r="C14" s="3"/>
       <c r="D14" s="8"/>
@@ -1128,19 +1124,19 @@
       </c>
       <c r="C15" s="3"/>
       <c r="D15" s="3" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="E15" s="3" t="s">
         <v>48</v>
       </c>
       <c r="F15" s="3"/>
       <c r="G15" s="3" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="H15" s="3"/>
       <c r="I15" s="3"/>
       <c r="J15" s="3" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="K15" s="5"/>
     </row>
@@ -1151,18 +1147,18 @@
       <c r="C16" s="3"/>
       <c r="D16" s="3"/>
       <c r="E16" s="4" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="F16" s="3" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="G16" s="3"/>
       <c r="H16" s="9" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="I16" s="3"/>
       <c r="J16" s="3" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="K16" s="5"/>
     </row>
@@ -1172,16 +1168,16 @@
       </c>
       <c r="C17" s="3"/>
       <c r="D17" s="3" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="E17" s="3"/>
       <c r="F17" s="3"/>
       <c r="G17" s="4" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="H17" s="3"/>
       <c r="I17" s="4" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="J17" s="9"/>
       <c r="K17" s="5"/>
@@ -1210,7 +1206,7 @@
       <c r="D19" s="3"/>
       <c r="E19" s="3"/>
       <c r="F19" s="10" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="G19" s="3"/>
       <c r="H19" s="3"/>
@@ -1224,12 +1220,12 @@
       </c>
       <c r="C20" s="3"/>
       <c r="D20" s="1" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="E20" s="3"/>
       <c r="F20" s="3"/>
       <c r="G20" s="1" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="H20" s="3"/>
       <c r="I20" s="3"/>
@@ -1251,7 +1247,7 @@
     </row>
     <row r="22" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B22" s="12" t="s">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="C22" s="13"/>
       <c r="D22" s="13"/>
@@ -1271,19 +1267,19 @@
     </row>
     <row r="24" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B24" s="11" t="s">
+        <v>70</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="E24" s="16" t="s">
+        <v>71</v>
+      </c>
+      <c r="G24" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="I24" s="1" t="s">
         <v>73</v>
-      </c>
-      <c r="D24" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="E24" s="16" t="s">
-        <v>74</v>
-      </c>
-      <c r="G24" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="I24" s="1" t="s">
-        <v>76</v>
       </c>
       <c r="K24" s="15"/>
     </row>
@@ -1320,7 +1316,7 @@
         <v>18</v>
       </c>
       <c r="C27" s="24" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="D27" s="24"/>
       <c r="E27" s="24"/>
@@ -1330,7 +1326,7 @@
       <c r="I27" s="24"/>
       <c r="J27" s="24"/>
       <c r="K27" s="25" t="s">
-        <v>84</v>
+        <v>78</v>
       </c>
     </row>
     <row r="28" spans="2:11" x14ac:dyDescent="0.25">
@@ -1338,7 +1334,7 @@
         <v>19</v>
       </c>
       <c r="C28" s="26" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="D28" s="26"/>
       <c r="E28" s="26"/>
@@ -1348,7 +1344,7 @@
       <c r="I28" s="26"/>
       <c r="J28" s="30"/>
       <c r="K28" s="31" t="s">
-        <v>84</v>
+        <v>78</v>
       </c>
     </row>
     <row r="29" spans="2:11" x14ac:dyDescent="0.25">
@@ -1356,7 +1352,7 @@
         <v>20</v>
       </c>
       <c r="C29" s="26" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
       <c r="D29" s="26"/>
       <c r="E29" s="26"/>
@@ -1366,7 +1362,7 @@
       <c r="I29" s="26"/>
       <c r="J29" s="30"/>
       <c r="K29" s="31" t="s">
-        <v>84</v>
+        <v>78</v>
       </c>
     </row>
     <row r="30" spans="2:11" x14ac:dyDescent="0.25">
@@ -1374,7 +1370,7 @@
         <v>21</v>
       </c>
       <c r="C30" s="26" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
       <c r="D30" s="26"/>
       <c r="E30" s="26"/>
@@ -1384,7 +1380,7 @@
       <c r="I30" s="26"/>
       <c r="J30" s="26"/>
       <c r="K30" s="31" t="s">
-        <v>84</v>
+        <v>78</v>
       </c>
     </row>
     <row r="31" spans="2:11" x14ac:dyDescent="0.25">
@@ -1392,7 +1388,7 @@
         <v>22</v>
       </c>
       <c r="C31" s="26" t="s">
-        <v>88</v>
+        <v>82</v>
       </c>
       <c r="D31" s="26"/>
       <c r="E31" s="26"/>
@@ -1402,13 +1398,13 @@
       <c r="I31" s="26"/>
       <c r="J31" s="26"/>
       <c r="K31" s="31" t="s">
-        <v>84</v>
+        <v>78</v>
       </c>
     </row>
     <row r="32" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B32" s="21"/>
       <c r="C32" s="26" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="D32" s="26"/>
       <c r="E32" s="26"/>
@@ -1424,7 +1420,7 @@
         <v>23</v>
       </c>
       <c r="C33" s="26" t="s">
-        <v>90</v>
+        <v>84</v>
       </c>
       <c r="D33" s="26"/>
       <c r="E33" s="26"/>
@@ -1434,7 +1430,7 @@
       <c r="I33" s="26"/>
       <c r="J33" s="26"/>
       <c r="K33" s="31" t="s">
-        <v>84</v>
+        <v>78</v>
       </c>
     </row>
     <row r="34" spans="2:11" x14ac:dyDescent="0.25">
@@ -1480,7 +1476,7 @@
       <c r="I36" s="26"/>
       <c r="J36" s="26"/>
       <c r="K36" s="31" t="s">
-        <v>92</v>
+        <v>86</v>
       </c>
     </row>
     <row r="37" spans="2:11" x14ac:dyDescent="0.25">
@@ -1502,7 +1498,7 @@
         <v>29</v>
       </c>
       <c r="C38" s="26" t="s">
-        <v>91</v>
+        <v>85</v>
       </c>
       <c r="D38" s="26"/>
       <c r="E38" s="26"/>
@@ -1512,7 +1508,7 @@
       <c r="I38" s="26"/>
       <c r="J38" s="26"/>
       <c r="K38" s="31" t="s">
-        <v>92</v>
+        <v>86</v>
       </c>
     </row>
     <row r="39" spans="2:11" x14ac:dyDescent="0.25">
@@ -1544,7 +1540,7 @@
       <c r="I40" s="29"/>
       <c r="J40" s="29"/>
       <c r="K40" s="31" t="s">
-        <v>92</v>
+        <v>86</v>
       </c>
     </row>
     <row r="41" spans="2:11" x14ac:dyDescent="0.25">
@@ -1617,7 +1613,7 @@
     </row>
     <row r="47" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B47" s="12" t="s">
-        <v>80</v>
+        <v>89</v>
       </c>
       <c r="C47" s="13"/>
       <c r="D47" s="13"/>
@@ -1631,13 +1627,13 @@
     </row>
     <row r="48" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B48" s="11" t="s">
-        <v>81</v>
+        <v>90</v>
       </c>
       <c r="K48" s="15"/>
     </row>
     <row r="49" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B49" s="11" t="s">
-        <v>82</v>
+        <v>91</v>
       </c>
       <c r="C49" s="23"/>
       <c r="K49" s="15"/>

</xml_diff>